<commit_message>
First commit towards POM framework
</commit_message>
<xml_diff>
--- a/src/main/java/com/qa/testdata/Data.xlsx
+++ b/src/main/java/com/qa/testdata/Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/k-bhatt/eclipse-workspace1/JavaSelenium/src/main/java/com/qa/testdata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/k-bhatt/eclipse-workspace1/POM_Selenium/src/main/java/com/qa/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E37E0A49-FB56-0247-952A-7DFB590ECF25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2C69FB1-195A-C04F-8F14-F69B45AF606F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4940" yWindow="1920" windowWidth="28040" windowHeight="17440" xr2:uid="{73C089CA-350C-434F-AE38-AEE6575881B6}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{51DB696F-2331-564B-808E-3D8FD6DCEE79}"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
@@ -25,69 +25,177 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="49">
+  <si>
+    <t>LoanRegistrationTest</t>
+  </si>
   <si>
     <t>Runmode</t>
   </si>
   <si>
-    <t>username</t>
-  </si>
-  <si>
-    <t>password</t>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>loan</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>firstname</t>
+  </si>
+  <si>
+    <t>lastname</t>
+  </si>
+  <si>
+    <t>day</t>
+  </si>
+  <si>
+    <t>month</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>income</t>
+  </si>
+  <si>
+    <t>home</t>
+  </si>
+  <si>
+    <t>rent</t>
+  </si>
+  <si>
+    <t>jobtitle</t>
+  </si>
+  <si>
+    <t>empname</t>
+  </si>
+  <si>
+    <t>empindustry</t>
+  </si>
+  <si>
+    <t>postcode</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>daymonth</t>
+  </si>
+  <si>
+    <t>dayyear</t>
+  </si>
+  <si>
+    <t>kebijebi@gmail.com</t>
+  </si>
+  <si>
+    <t>Mr</t>
+  </si>
+  <si>
+    <t>Kartik</t>
+  </si>
+  <si>
+    <t>Bhatt</t>
+  </si>
+  <si>
+    <t>Employed full-time</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>software engineer</t>
+  </si>
+  <si>
+    <t>Equiis</t>
+  </si>
+  <si>
+    <t>Computers - Software</t>
+  </si>
+  <si>
+    <t>BT2 8EP</t>
+  </si>
+  <si>
+    <t>March</t>
+  </si>
+  <si>
+    <t>Car</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>1984</t>
+  </si>
+  <si>
+    <t>65000</t>
+  </si>
+  <si>
+    <t>1200</t>
+  </si>
+  <si>
+    <t>1987</t>
+  </si>
+  <si>
+    <t>Flat 54, Bass Buildings, 38 Alfred Street, Belfast, BT2 8EP</t>
+  </si>
+  <si>
+    <t>EmailValidationTest</t>
   </si>
   <si>
     <t>errorMsg</t>
   </si>
   <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>Epic sadface: Username is required</t>
-  </si>
-  <si>
-    <t>secret_sauce</t>
-  </si>
-  <si>
-    <t>standard_user</t>
-  </si>
-  <si>
-    <t>Epic sadface: Password is required</t>
-  </si>
-  <si>
-    <t>locked_out_user</t>
-  </si>
-  <si>
-    <t>Epic sadface: Sorry, this user has been locked out.</t>
-  </si>
-  <si>
-    <t>Tes123</t>
-  </si>
-  <si>
-    <t>Epic sadface: Username and password do not match any user in this service</t>
-  </si>
-  <si>
-    <t>test123</t>
-  </si>
-  <si>
-    <t>problem_user</t>
-  </si>
-  <si>
-    <t>performance_glitch_user</t>
-  </si>
-  <si>
-    <t>IncorrectLoginTest</t>
-  </si>
-  <si>
-    <t>CorrectLoginTest</t>
+    <t>Oops, this can't be blank</t>
+  </si>
+  <si>
+    <t>kebijebi</t>
+  </si>
+  <si>
+    <t>Oops, that doesn't look quite right. Please check your email address.</t>
+  </si>
+  <si>
+    <t>PostcodeValidationTest</t>
+  </si>
+  <si>
+    <t>Oops, this postcode doesn't look quite right</t>
+  </si>
+  <si>
+    <t>123</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -103,13 +211,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -123,15 +231,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -443,162 +558,229 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7C02850-5E65-A542-843A-FF8FFC549091}">
-  <dimension ref="A1:D14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58425118-14AE-4243-8982-D541DF6B6403}">
+  <dimension ref="A1:T13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" zoomScale="117" zoomScaleNormal="117" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="21.1640625" customWidth="1"/>
-    <col min="2" max="2" width="22.1640625" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" customWidth="1"/>
-    <col min="4" max="4" width="64.83203125" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:20" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="O2" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="P2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="J3" t="s">
+        <v>26</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="L3" t="s">
+        <v>27</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="N3" t="s">
+        <v>28</v>
+      </c>
+      <c r="O3" t="s">
+        <v>29</v>
+      </c>
+      <c r="P3" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>31</v>
+      </c>
+      <c r="R3" t="s">
+        <v>40</v>
+      </c>
+      <c r="S3" t="s">
+        <v>32</v>
+      </c>
+      <c r="T3" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" ht="21" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="5"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="B6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C7" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>44</v>
       </c>
       <c r="C8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B11" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" ht="21" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" s="5"/>
+      <c r="C10" s="2"/>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="B11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>4</v>
-      </c>
-      <c r="B12" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C12" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13" t="s">
-        <v>14</v>
+        <v>2</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>48</v>
       </c>
       <c r="C13" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>4</v>
-      </c>
-      <c r="B14" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" t="s">
-        <v>6</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C12:F12"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="C3" r:id="rId1" xr:uid="{44760532-F20D-D54B-9868-5532AA200DD3}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>